<commit_message>
Fixed Pawn Generate - 3270351598 업데이트
</commit_message>
<xml_diff>
--- a/Data/Fixed Pawn Generate - 3270351598/3270351598.xlsx
+++ b/Data/Fixed Pawn Generate - 3270351598/3270351598.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bjmi0\Desktop\림월드 번역\Fixed Pawn Generate - 3270351598\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13FC4284-0D8A-467C-9081-B2E69AE0E2B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99FA6AB0-1036-4DE5-9303-62F556CB3B51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,8 +19,44 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>bjmi0</author>
+  </authors>
+  <commentList>
+    <comment ref="E8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2024-12-20에 새로 추가된 노드들 (23개)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F8" authorId="0" shapeId="0" xr:uid="{E003C66F-2430-4413-8458-5E63044DBF96}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2024-12-20에 새로 추가된 노드들 (23개)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="107">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -55,21 +91,45 @@
     <t>Keyed+allowRelationDescription</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>자연스러운 관계 생성 허용</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>allowRelationDescription</t>
   </si>
   <si>
+    <t>maxGenerateRate_Starting</t>
+  </si>
+  <si>
     <t>Keyed+maxGenerateRate_Starting</t>
   </si>
   <si>
-    <t>maxGenerateRate_Starting</t>
-  </si>
-  <si>
     <t>Highest generation rate for custom characters in the starting character selection screen: {0}</t>
   </si>
   <si>
     <t>Keyed+maxGenerateRate_Global</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>시작 캐릭터 선택 화면에서 커스텀 캐릭터 등장 확률: {0}</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>maxGenerateRate_Global</t>
   </si>
   <si>
@@ -79,22 +139,294 @@
     <t>Keyed+Reset</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>인간 생성 시 커스텀 캐릭터 등장 확률: {0}</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>Reset</t>
   </si>
   <si>
-    <t>초기화</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>자연스러운 관계 생성 허용</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>인간 생성 시 커스텀 캐릭터 등장 확률: {0}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>시작 캐릭터 선택 화면에서 커스텀 캐릭터 등장 확률: {0}</t>
+    <t>FixedPawnGenerate.FixedPawnDef+TestAlianPawn1.firstName</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>초기화</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>FixedPawnGenerate.FixedPawnDef</t>
+  </si>
+  <si>
+    <t>TestAlianPawn1.firstName</t>
+  </si>
+  <si>
+    <t>TestFirstName</t>
+  </si>
+  <si>
+    <t>FixedPawnGenerate.FixedPawnDef+TestAlianPawn1.nickName</t>
+  </si>
+  <si>
+    <t>TestAlianPawn1.nickName</t>
+  </si>
+  <si>
+    <t>TestAlian</t>
+  </si>
+  <si>
+    <t>FixedPawnGenerate.FixedPawnDef+TestAlianPawn1.lastName</t>
+  </si>
+  <si>
+    <t>TestAlianPawn1.lastName</t>
+  </si>
+  <si>
+    <t>TestLastName</t>
+  </si>
+  <si>
+    <t>FixedPawnGenerate.FixedPawnDef+TestPawn1.firstName</t>
+  </si>
+  <si>
+    <t>TestPawn1.firstName</t>
+  </si>
+  <si>
+    <t>FixedPawnGenerate.FixedPawnDef+TestPawn1.nickName</t>
+  </si>
+  <si>
+    <t>TestPawn1.nickName</t>
+  </si>
+  <si>
+    <t>TestNickName</t>
+  </si>
+  <si>
+    <t>FixedPawnGenerate.FixedPawnDef+TestPawn1.lastName</t>
+  </si>
+  <si>
+    <t>TestPawn1.lastName</t>
+  </si>
+  <si>
+    <t>FixedPawnGenerate.FixedPawnDef+TestParent.firstName</t>
+  </si>
+  <si>
+    <t>TestParent.firstName</t>
+  </si>
+  <si>
+    <t>TestParent</t>
+  </si>
+  <si>
+    <t>FixedPawnGenerate.FixedPawnDef+TestParent.nickName</t>
+  </si>
+  <si>
+    <t>TestParent.nickName</t>
+  </si>
+  <si>
+    <t>FixedPawnGenerate.FixedPawnDef+TestParent.lastName</t>
+  </si>
+  <si>
+    <t>TestParent.lastName</t>
+  </si>
+  <si>
+    <t>FixedPawnGenerate.FixedPawnDef+WSGR_Lexingtontest.firstName</t>
+  </si>
+  <si>
+    <t>WSGR_Lexingtontest.firstName</t>
+  </si>
+  <si>
+    <t>航母</t>
+  </si>
+  <si>
+    <t>FixedPawnGenerate.FixedPawnDef+WSGR_Lexingtontest.nickName</t>
+  </si>
+  <si>
+    <t>WSGR_Lexingtontest.nickName</t>
+  </si>
+  <si>
+    <t>列克星敦</t>
+  </si>
+  <si>
+    <t>FixedPawnGenerate.FixedPawnDef+WSGR_Lexingtontest.lastName</t>
+  </si>
+  <si>
+    <t>WSGR_Lexingtontest.lastName</t>
+  </si>
+  <si>
+    <t>舰娘</t>
+  </si>
+  <si>
+    <t>ScenPartDef+ConfigPage_ConfigureStartingFixedPawns.label</t>
+  </si>
+  <si>
+    <t>ScenPartDef</t>
+  </si>
+  <si>
+    <t>ConfigPage_ConfigureStartingFixedPawns.label</t>
+  </si>
+  <si>
+    <t>starting fixed pawns</t>
+  </si>
+  <si>
+    <t>Keyed+FPG_Generate</t>
+  </si>
+  <si>
+    <t>FPG_Generate</t>
+  </si>
+  <si>
+    <t>Character Generation</t>
+  </si>
+  <si>
+    <t>Keyed+FPG_Protrait</t>
+  </si>
+  <si>
+    <t>FPG_Protrait</t>
+  </si>
+  <si>
+    <t>Portrait Control</t>
+  </si>
+  <si>
+    <t>Keyed+FPG_allowMainProtrait</t>
+  </si>
+  <si>
+    <t>FPG_allowMainProtrait</t>
+  </si>
+  <si>
+    <t>Enable Main Portrait</t>
+  </si>
+  <si>
+    <t>Keyed+FPG_allowMainProtrait_description</t>
+  </si>
+  <si>
+    <t>FPG_allowMainProtrait_description</t>
+  </si>
+  <si>
+    <t>The portrait in the lower left corner of the game interface</t>
+  </si>
+  <si>
+    <t>Keyed+FPG_allowInfoProtrait</t>
+  </si>
+  <si>
+    <t>FPG_allowInfoProtrait</t>
+  </si>
+  <si>
+    <t>Enable Attribute Panel Portrait</t>
+  </si>
+  <si>
+    <t>Keyed+FPG_allowInfoProtrait_description</t>
+  </si>
+  <si>
+    <t>FPG_allowInfoProtrait_description</t>
+  </si>
+  <si>
+    <t>The portrait in the character attribute panel</t>
+  </si>
+  <si>
+    <t>Keyed+FPG_showFullProtrait</t>
+  </si>
+  <si>
+    <t>FPG_showFullProtrait</t>
+  </si>
+  <si>
+    <t>Show Full-Body Portrait</t>
+  </si>
+  <si>
+    <t>Keyed+FPG_showFullProtrait_description</t>
+  </si>
+  <si>
+    <t>FPG_showFullProtrait_description</t>
+  </si>
+  <si>
+    <t>Enable full-body portrait, disabled by default</t>
+  </si>
+  <si>
+    <t>Keyed+FPG_globalProtraitOffsetY</t>
+  </si>
+  <si>
+    <t>FPG_globalProtraitOffsetY</t>
+  </si>
+  <si>
+    <t>Portrait Vertical Offset</t>
+  </si>
+  <si>
+    <t>Keyed+FPG_globalProtraitOffsetY_description</t>
+  </si>
+  <si>
+    <t>FPG_globalProtraitOffsetY_description</t>
+  </si>
+  <si>
+    <t>Vertical offset of the portrait, negative values move it upwards</t>
+  </si>
+  <si>
+    <t>테스트 성</t>
+  </si>
+  <si>
+    <t>테스트 성</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>테스트 별명</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>테스트 이름</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>테스트 부모</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>캐릭터 생성</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>초상화 설정</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>캐릭터 정보창의 초상화를 활성화합니다</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>게임 UI 왼쪽 하단 초상화를 활성화합니다</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>정보창 초상화 활성화</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>메인 초상화 활성화</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>전신 초상화 표시</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>초상화에 전신을 표시합니다(기본적으로 비활성화됨)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>초상화 위치 설정</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>세로 위치를 조절합니다. 음수 값을 넣으면 위로 이동합니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>커스텀 캐릭터로 게임 시작</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -102,7 +434,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -121,13 +453,24 @@
       <family val="3"/>
       <charset val="129"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF87CEEB"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -142,9 +485,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -446,17 +790,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="7" width="9.1796875" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.1796875" style="1"/>
+    <col min="1" max="1" width="9.1796875" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
@@ -493,7 +837,7 @@
         <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -504,18 +848,18 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
@@ -524,48 +868,440 @@
         <v>13</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A21" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A22" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A23" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A25" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A26" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A27" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A28" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A29" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A30" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>